<commit_message>
Add new metadata sheet
</commit_message>
<xml_diff>
--- a/src/flo/homeassistant/src/build/resources/entity_metadata.xlsx
+++ b/src/flo/homeassistant/src/build/resources/entity_metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/graham/Code/asystem/src/flo/homeassistant/src/build/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA8C7234-0C08-954F-815F-41BD536D3286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCDC4CC-7F56-A24A-B5E3-71601965B4EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="1760" windowWidth="41120" windowHeight="24740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5638,8 +5638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AY724"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AK254" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="AM278" sqref="AM278"/>
+    <sheetView tabSelected="1" topLeftCell="A254" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="A276" sqref="A276"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" customHeight="1"/>

</xml_diff>